<commit_message>
version final del eda
</commit_message>
<xml_diff>
--- a/Aux_Tecnicos.xlsx
+++ b/Aux_Tecnicos.xlsx
@@ -367,17 +367,17 @@
     <row r="1" s="1" customFormat="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Año</t>
+          <t>MYEAR</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Selección</t>
+          <t>Seleccion</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Nombre del Entrenador</t>
+          <t>COACH</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">

</xml_diff>